<commit_message>
fix: for class presentation
</commit_message>
<xml_diff>
--- a/sql/sample-data.xlsx
+++ b/sql/sample-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ttontoey/Documents/db-sys-bookbook/sql/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F88D498-505D-3547-9A16-F0F6B92B258F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F2CC269-9631-044E-A2E3-AE5868AB01D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{F431DE53-69A8-9647-BE0C-224C100AC897}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" firstSheet="4" activeTab="6" xr2:uid="{F431DE53-69A8-9647-BE0C-224C100AC897}"/>
   </bookViews>
   <sheets>
     <sheet name="userinformation" sheetId="21" r:id="rId1"/>
@@ -26,14 +26,15 @@
     <sheet name="booktag" sheetId="11" r:id="rId11"/>
     <sheet name="specialdescription" sheetId="13" r:id="rId12"/>
     <sheet name="damage" sheetId="14" r:id="rId13"/>
-    <sheet name="book" sheetId="9" r:id="rId14"/>
-    <sheet name="sellpost" sheetId="12" r:id="rId15"/>
-    <sheet name="transaction" sheetId="15" r:id="rId16"/>
-    <sheet name="payment" sheetId="17" r:id="rId17"/>
-    <sheet name="evidence" sheetId="16" r:id="rId18"/>
-    <sheet name="shipment" sheetId="18" r:id="rId19"/>
-    <sheet name="searchhistory" sheetId="19" r:id="rId20"/>
-    <sheet name="message" sheetId="20" r:id="rId21"/>
+    <sheet name="Sheet2" sheetId="23" r:id="rId14"/>
+    <sheet name="book" sheetId="9" r:id="rId15"/>
+    <sheet name="sellpost" sheetId="12" r:id="rId16"/>
+    <sheet name="transaction" sheetId="15" r:id="rId17"/>
+    <sheet name="payment" sheetId="17" r:id="rId18"/>
+    <sheet name="evidence" sheetId="16" r:id="rId19"/>
+    <sheet name="shipment" sheetId="18" r:id="rId20"/>
+    <sheet name="searchhistory" sheetId="19" r:id="rId21"/>
+    <sheet name="message" sheetId="20" r:id="rId22"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -1429,7 +1430,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45D67B75-98A3-3A42-9533-87172308BA2F}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
@@ -2170,7 +2171,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2207,6 +2208,18 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C5FB002-B3F4-2546-B152-F114059A6A04}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90B177C0-130C-ED49-AFE8-3D1705AB6953}">
   <dimension ref="A1:L12"/>
   <sheetViews>
@@ -2688,7 +2701,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82BF8082-BFB1-0A44-AB0E-04E157F29C00}">
   <dimension ref="A1:G23"/>
   <sheetViews>
@@ -2907,7 +2920,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35092F04-8AB1-5542-8E1E-C036E832A375}">
   <dimension ref="A1:I16"/>
   <sheetViews>
@@ -3081,7 +3094,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92718C27-8B02-8045-A2D7-FF1ABDC52011}">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -3168,7 +3181,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AF1321F-EE90-4148-A6C8-C22E5449D41F}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -3212,93 +3225,6 @@
       </c>
       <c r="B4" s="2" t="s">
         <v>58</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BD335A9-7158-F04B-A211-9B5A45EC1C02}">
-  <dimension ref="A1:E4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="19.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>269</v>
-      </c>
-      <c r="B1" t="s">
-        <v>217</v>
-      </c>
-      <c r="C1" t="s">
-        <v>228</v>
-      </c>
-      <c r="D1" t="s">
-        <v>224</v>
-      </c>
-      <c r="E1" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>295</v>
       </c>
     </row>
   </sheetData>
@@ -3610,6 +3536,93 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BD335A9-7158-F04B-A211-9B5A45EC1C02}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="19.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C1" t="s">
+        <v>228</v>
+      </c>
+      <c r="D1" t="s">
+        <v>224</v>
+      </c>
+      <c r="E1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E147E3A-BB3A-F34C-90FA-1985554C94F6}">
   <dimension ref="A1:B24"/>
   <sheetViews>
@@ -3819,7 +3832,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28C78963-1353-8046-9C2D-C8E136DEA44C}">
   <dimension ref="A1:I9"/>
   <sheetViews>
@@ -5290,7 +5303,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45597351-1F61-5A4E-A3EE-C66ACF6231A8}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>

</xml_diff>